<commit_message>
Add teacher finished, and sheet update
</commit_message>
<xml_diff>
--- a/Planilha esperada.xlsx
+++ b/Planilha esperada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tulio\Desktop\-\Projetos programação\Horarios-CEFET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83F6C4-6823-49AF-B8E4-319554B9606B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F726F1BD-9B32-4188-B1C5-3E2B2B7B36DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="1050" windowWidth="16710" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Tulio</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Professor</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Matéria</t>
   </si>
   <si>
-    <t>Tipo de matéria</t>
-  </si>
-  <si>
-    <t>Número de grupos</t>
-  </si>
-  <si>
     <t>Preferências</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Desenho Técnico</t>
   </si>
   <si>
-    <t>Anual</t>
-  </si>
-  <si>
     <t>S3-N2-N6</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>Robótica integrada</t>
   </si>
   <si>
-    <t>Bimestral</t>
-  </si>
-  <si>
     <t>N1bm-S6</t>
   </si>
   <si>
@@ -145,6 +133,9 @@
   </si>
   <si>
     <t>A parte verde é o número de aulas por semana que ele dá daquela determinada matéria para cada turma</t>
+  </si>
+  <si>
+    <t>Limitações</t>
   </si>
 </sst>
 </file>
@@ -522,19 +513,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="5" width="17.85546875" customWidth="1"/>
+    <col min="2" max="4" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,168 +536,140 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3">
-        <v>3</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -717,7 +680,6 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -741,10 +703,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>